<commit_message>
updated readme question exclusion instructions
</commit_message>
<xml_diff>
--- a/ftr_questionnaire/drafts_e1_to_e4/questions.xlsx
+++ b/ftr_questionnaire/drafts_e1_to_e4/questions.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cole/Dropbox/ftr_research/ftr_questionnaire_master/ftr_questionnaire/drafts_e1_to_e4/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4ACB76-9D4F-A047-8563-C574E262DF89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="27160" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -609,8 +615,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +679,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -719,7 +733,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -751,9 +765,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -785,6 +817,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -960,14 +1010,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1075,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1076,7 +1128,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1129,7 +1181,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1182,7 +1234,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1235,7 +1287,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1288,7 +1340,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1341,7 +1393,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1394,7 +1446,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1447,7 +1499,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1500,7 +1552,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1553,7 +1605,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1606,7 +1658,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1659,7 +1711,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1712,7 +1764,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1765,7 +1817,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1818,7 +1870,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1871,7 +1923,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1924,7 +1976,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1977,7 +2029,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2030,7 +2082,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2083,7 +2135,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2136,7 +2188,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2189,7 +2241,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2242,7 +2294,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2295,7 +2347,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2348,7 +2400,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2401,7 +2453,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2454,7 +2506,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2507,7 +2559,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2560,7 +2612,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2613,7 +2665,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2666,7 +2718,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2719,7 +2771,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2772,7 +2824,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2825,7 +2877,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2878,7 +2930,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2931,7 +2983,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2987,7 +3039,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -3043,7 +3095,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -3099,7 +3151,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -3152,7 +3204,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3205,7 +3257,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3258,7 +3310,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3311,7 +3363,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3364,7 +3416,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3417,7 +3469,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -3470,7 +3522,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3523,7 +3575,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
@@ -3576,7 +3628,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -3629,7 +3681,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2</v>
       </c>
@@ -3682,7 +3734,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -3735,7 +3787,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3788,7 +3840,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -3841,7 +3893,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -3894,7 +3946,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2</v>
       </c>
@@ -3947,7 +3999,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2</v>
       </c>
@@ -4000,7 +4052,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2</v>
       </c>
@@ -4053,7 +4105,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -4106,7 +4158,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2</v>
       </c>
@@ -4159,7 +4211,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2</v>
       </c>
@@ -4212,7 +4264,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2</v>
       </c>
@@ -4265,7 +4317,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2</v>
       </c>
@@ -4318,7 +4370,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2</v>
       </c>
@@ -4371,7 +4423,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2</v>
       </c>
@@ -4424,7 +4476,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2</v>
       </c>
@@ -4477,7 +4529,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2</v>
       </c>
@@ -4530,7 +4582,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2</v>
       </c>
@@ -4583,7 +4635,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2</v>
       </c>
@@ -4636,7 +4688,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2</v>
       </c>
@@ -4689,7 +4741,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2</v>
       </c>
@@ -4742,7 +4794,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2</v>
       </c>
@@ -4795,7 +4847,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2</v>
       </c>
@@ -4848,7 +4900,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2</v>
       </c>
@@ -4901,7 +4953,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2</v>
       </c>
@@ -4954,7 +5006,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2</v>
       </c>
@@ -5007,7 +5059,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2</v>
       </c>
@@ -5060,7 +5112,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2</v>
       </c>
@@ -5113,7 +5165,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2</v>
       </c>
@@ -5166,7 +5218,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2</v>
       </c>
@@ -5219,7 +5271,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2</v>
       </c>
@@ -5272,7 +5324,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2</v>
       </c>
@@ -5325,7 +5377,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2</v>
       </c>
@@ -5378,7 +5430,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2</v>
       </c>
@@ -5431,7 +5483,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2</v>
       </c>
@@ -5484,7 +5536,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2</v>
       </c>
@@ -5540,7 +5592,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2</v>
       </c>
@@ -5596,7 +5648,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2</v>
       </c>
@@ -5652,7 +5704,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2</v>
       </c>
@@ -5705,7 +5757,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2</v>
       </c>
@@ -5758,7 +5810,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2</v>
       </c>
@@ -5811,7 +5863,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2</v>
       </c>
@@ -5864,7 +5916,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2</v>
       </c>
@@ -5917,7 +5969,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2</v>
       </c>
@@ -5970,7 +6022,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2</v>
       </c>
@@ -6023,7 +6075,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2</v>
       </c>
@@ -6076,7 +6128,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2</v>
       </c>
@@ -6129,7 +6181,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>3</v>
       </c>
@@ -6182,7 +6234,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>3</v>
       </c>
@@ -6235,7 +6287,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>3</v>
       </c>
@@ -6288,7 +6340,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>3</v>
       </c>
@@ -6341,7 +6393,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>3</v>
       </c>
@@ -6394,7 +6446,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>3</v>
       </c>
@@ -6447,7 +6499,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>3</v>
       </c>
@@ -6500,7 +6552,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>3</v>
       </c>
@@ -6553,7 +6605,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>3</v>
       </c>
@@ -6606,7 +6658,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>3</v>
       </c>
@@ -6659,7 +6711,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>3</v>
       </c>
@@ -6712,7 +6764,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>3</v>
       </c>
@@ -6765,7 +6817,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>3</v>
       </c>
@@ -6818,7 +6870,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>3</v>
       </c>
@@ -6871,7 +6923,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>3</v>
       </c>
@@ -6924,7 +6976,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="113" spans="1:18">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>3</v>
       </c>
@@ -6977,7 +7029,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="114" spans="1:18">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>3</v>
       </c>
@@ -7030,7 +7082,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="115" spans="1:18">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>3</v>
       </c>
@@ -7083,7 +7135,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="116" spans="1:18">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>3</v>
       </c>
@@ -7136,7 +7188,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="117" spans="1:18">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>3</v>
       </c>
@@ -7189,7 +7241,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="118" spans="1:18">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>3</v>
       </c>
@@ -7242,7 +7294,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="119" spans="1:18">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>3</v>
       </c>
@@ -7295,7 +7347,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="120" spans="1:18">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>3</v>
       </c>
@@ -7348,7 +7400,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="121" spans="1:18">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>3</v>
       </c>
@@ -7401,7 +7453,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="122" spans="1:18">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>3</v>
       </c>
@@ -7454,7 +7506,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="123" spans="1:18">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>3</v>
       </c>
@@ -7507,7 +7559,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="124" spans="1:18">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>3</v>
       </c>
@@ -7560,7 +7612,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="125" spans="1:18">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>3</v>
       </c>
@@ -7613,7 +7665,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="126" spans="1:18">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>3</v>
       </c>
@@ -7666,7 +7718,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="127" spans="1:18">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>3</v>
       </c>
@@ -7719,7 +7771,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="128" spans="1:18">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>3</v>
       </c>
@@ -7772,7 +7824,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="129" spans="1:18">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>3</v>
       </c>
@@ -7825,7 +7877,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="130" spans="1:18">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>3</v>
       </c>
@@ -7878,7 +7930,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="131" spans="1:18">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>3</v>
       </c>
@@ -7931,7 +7983,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="132" spans="1:18">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>3</v>
       </c>
@@ -7984,7 +8036,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="133" spans="1:18">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>3</v>
       </c>
@@ -8037,7 +8089,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="134" spans="1:18">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>3</v>
       </c>
@@ -8093,7 +8145,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="135" spans="1:18">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>3</v>
       </c>
@@ -8149,7 +8201,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="136" spans="1:18">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>3</v>
       </c>
@@ -8205,7 +8257,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="137" spans="1:18">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>3</v>
       </c>
@@ -8258,7 +8310,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="138" spans="1:18">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>3</v>
       </c>
@@ -8311,7 +8363,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="139" spans="1:18">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>3</v>
       </c>
@@ -8364,7 +8416,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="140" spans="1:18">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>3</v>
       </c>
@@ -8417,7 +8469,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="141" spans="1:18">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>3</v>
       </c>
@@ -8470,7 +8522,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="142" spans="1:18">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>3</v>
       </c>
@@ -8523,7 +8575,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="143" spans="1:18">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>3</v>
       </c>
@@ -8576,7 +8628,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="144" spans="1:18">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>3</v>
       </c>
@@ -8629,7 +8681,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:18">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>3</v>
       </c>

</xml_diff>